<commit_message>
Se modifica el excel con los atributos de la base de datos
</commit_message>
<xml_diff>
--- a/data/database/databaste_atributes.xlsx
+++ b/data/database/databaste_atributes.xlsx
@@ -1,16 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <workbookPr defaultThemeVersion="202300"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Universidad\MsC\VA\proyecto curso\database\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10D0591B-C029-4EAA-8564-204061D3BCAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet name="imagebase_division" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="imagebase_division" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="17">
   <si>
     <t>id</t>
   </si>
@@ -66,29 +76,24 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt formatCode="GENERAL" numFmtId="164"/>
-    <numFmt formatCode="DD/MM/YY" numFmtId="165"/>
-    <numFmt formatCode="DD/MM/YYYY\ HH:MM:SS" numFmtId="166"/>
-    <numFmt formatCode="HH:MM:SS" numFmtId="167"/>
-    <numFmt formatCode="DD/MM/YYYY\ HH:MM:SS.000" numFmtId="168"/>
-    <numFmt formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;" numFmtId="169"/>
-  </numFmts>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <sz val="10"/>
     </font>
   </fonts>
-  <fills count="1">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
+    <fill>
+      <patternFill patternType="gray125"/>
+    </fill>
   </fills>
   <borders count="1">
-    <border diagonalDown="false" diagonalUp="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -97,35 +102,377 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="164">
-</xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
-    <xf numFmtId="164" xfId="0"/>
-    <xf numFmtId="165" xfId="0"/>
-    <xf numFmtId="166" xfId="0"/>
-    <xf numFmtId="167" xfId="0"/>
-    <xf numFmtId="168" xfId="0"/>
-    <xf numFmtId="169" xfId="0"/>
+  <cellXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E4AF26D0-793E-41E4-BDA4-36781804406B}" name="Tabla1" displayName="Tabla1" ref="A1:F23" totalsRowShown="0">
+  <autoFilter ref="A1:F23" xr:uid="{E4AF26D0-793E-41E4-BDA4-36781804406B}">
+    <filterColumn colId="5">
+      <filters>
+        <filter val="train"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{16E9492E-8D29-4D3A-95A5-46A4CB5D6F00}" name="id"/>
+    <tableColumn id="2" xr3:uid="{4CBF846D-53A5-4305-8932-273D34650528}" name="grass_type"/>
+    <tableColumn id="3" xr3:uid="{05B55C66-E49E-48DF-9E08-964D9FC83836}" name="elev_type"/>
+    <tableColumn id="4" xr3:uid="{631A26F5-1046-4C0E-97BF-5AA64BEA2655}" name="crop"/>
+    <tableColumn id="5" xr3:uid="{039E1978-9DA7-472C-B88F-6D9D3C7951C7}" name="dev_stage"/>
+    <tableColumn id="6" xr3:uid="{64D5C9A5-C595-4208-BD81-4DE95D9C914C}" name="split"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="0E2841"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E8E8E8"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="156082"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="E97132"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="196B24"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="0F9ED5"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="A02B93"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="4EA72E"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="467886"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="96607D"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1024" width="15"/>
-    <col min="2" max="1024" width="15"/>
-    <col min="3" max="1024" width="15"/>
-    <col min="4" max="1024" width="15"/>
-    <col min="5" max="1024" width="15"/>
-    <col min="6" max="1024" width="15"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -145,29 +492,29 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3">
-        <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -185,49 +532,49 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5">
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6">
-        <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
@@ -245,9 +592,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:6" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
@@ -265,9 +612,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
@@ -285,9 +632,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:6" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
         <v>12</v>
@@ -305,9 +652,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
         <v>12</v>
@@ -325,9 +672,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:6" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
         <v>12</v>
@@ -345,9 +692,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" t="s">
         <v>12</v>
@@ -365,9 +712,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" t="s">
         <v>8</v>
@@ -385,9 +732,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" t="s">
         <v>8</v>
@@ -405,9 +752,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15" t="s">
         <v>8</v>
@@ -425,9 +772,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:6" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16" t="s">
         <v>8</v>
@@ -445,9 +792,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17" t="s">
         <v>6</v>
@@ -465,9 +812,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:6" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18" t="s">
         <v>12</v>
@@ -485,9 +832,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:6" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19" t="s">
         <v>12</v>
@@ -505,49 +852,49 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" t="s">
+        <v>8</v>
+      </c>
+      <c r="F20" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A21">
         <v>19</v>
       </c>
-      <c r="B20" t="s">
-        <v>8</v>
-      </c>
-      <c r="C20" t="s">
-        <v>11</v>
-      </c>
-      <c r="D20" t="s">
-        <v>7</v>
-      </c>
-      <c r="E20" t="s">
-        <v>8</v>
-      </c>
-      <c r="F20" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21">
+      <c r="B21" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" t="s">
+        <v>14</v>
+      </c>
+      <c r="F21" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A22">
         <v>20</v>
-      </c>
-      <c r="B21" t="s">
-        <v>12</v>
-      </c>
-      <c r="C21" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21" t="s">
-        <v>15</v>
-      </c>
-      <c r="E21" t="s">
-        <v>14</v>
-      </c>
-      <c r="F21" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22">
-        <v>21</v>
       </c>
       <c r="B22" t="s">
         <v>12</v>
@@ -565,7 +912,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
@@ -586,5 +933,9 @@
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
se modifica estructura del repo y readme
</commit_message>
<xml_diff>
--- a/data/database/databaste_atributes.xlsx
+++ b/data/database/databaste_atributes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Universidad\MsC\VA\proyecto curso\database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Universidad\MsC\VA\proyecto curso\citrus3-detector\data\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10D0591B-C029-4EAA-8564-204061D3BCAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB500F45-4C36-4B46-8155-D3D5145439AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="imagebase_division" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="19">
   <si>
     <t>id</t>
   </si>
@@ -71,6 +71,12 @@
   </si>
   <si>
     <t>young</t>
+  </si>
+  <si>
+    <t>Area (m^2)</t>
+  </si>
+  <si>
+    <t>Area (Ha)</t>
   </si>
 </sst>
 </file>
@@ -124,21 +130,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E4AF26D0-793E-41E4-BDA4-36781804406B}" name="Tabla1" displayName="Tabla1" ref="A1:F23" totalsRowShown="0">
-  <autoFilter ref="A1:F23" xr:uid="{E4AF26D0-793E-41E4-BDA4-36781804406B}">
-    <filterColumn colId="5">
-      <filters>
-        <filter val="train"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
-  <tableColumns count="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E4AF26D0-793E-41E4-BDA4-36781804406B}" name="Tabla1" displayName="Tabla1" ref="A1:H23" totalsRowShown="0">
+  <autoFilter ref="A1:H23" xr:uid="{E4AF26D0-793E-41E4-BDA4-36781804406B}"/>
+  <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{16E9492E-8D29-4D3A-95A5-46A4CB5D6F00}" name="id"/>
     <tableColumn id="2" xr3:uid="{4CBF846D-53A5-4305-8932-273D34650528}" name="grass_type"/>
     <tableColumn id="3" xr3:uid="{05B55C66-E49E-48DF-9E08-964D9FC83836}" name="elev_type"/>
     <tableColumn id="4" xr3:uid="{631A26F5-1046-4C0E-97BF-5AA64BEA2655}" name="crop"/>
     <tableColumn id="5" xr3:uid="{039E1978-9DA7-472C-B88F-6D9D3C7951C7}" name="dev_stage"/>
     <tableColumn id="6" xr3:uid="{64D5C9A5-C595-4208-BD81-4DE95D9C914C}" name="split"/>
+    <tableColumn id="7" xr3:uid="{A3CE59BE-E757-4BEB-8615-30187CECCEB9}" name="Area (m^2)"/>
+    <tableColumn id="8" xr3:uid="{6641261E-4102-46D7-86DC-E62A29A71D42}" name="Area (Ha)"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -461,18 +463,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1024" width="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -491,8 +493,14 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -511,8 +519,14 @@
       <c r="F2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G2">
+        <v>5932.7340000000004</v>
+      </c>
+      <c r="H2">
+        <v>0.59299999999999997</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -531,8 +545,14 @@
       <c r="F3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="G3">
+        <v>9214.1880000000001</v>
+      </c>
+      <c r="H3">
+        <v>0.92100000000000004</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -551,8 +571,14 @@
       <c r="F4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="G4">
+        <v>9787.143</v>
+      </c>
+      <c r="H4">
+        <v>0.97899999999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -571,8 +597,14 @@
       <c r="F5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G5">
+        <v>5911.09</v>
+      </c>
+      <c r="H5">
+        <v>0.59099999999999997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -591,8 +623,14 @@
       <c r="F6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G6">
+        <v>6042.2740000000003</v>
+      </c>
+      <c r="H6">
+        <v>0.60399999999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -611,8 +649,14 @@
       <c r="F7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="G7">
+        <v>6122.893</v>
+      </c>
+      <c r="H7">
+        <v>0.61199999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -631,8 +675,14 @@
       <c r="F8" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G8">
+        <v>11559.834000000001</v>
+      </c>
+      <c r="H8">
+        <v>1.1559999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -651,8 +701,14 @@
       <c r="F9" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="G9">
+        <v>9116.0849999999991</v>
+      </c>
+      <c r="H9">
+        <v>0.91200000000000003</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -671,8 +727,14 @@
       <c r="F10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G10">
+        <v>9358.5400000000009</v>
+      </c>
+      <c r="H10">
+        <v>0.93600000000000005</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -691,8 +753,14 @@
       <c r="F11" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="G11">
+        <v>6912.3890000000001</v>
+      </c>
+      <c r="H11">
+        <v>0.69099999999999995</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -711,8 +779,14 @@
       <c r="F12" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="G12">
+        <v>9240.3279999999995</v>
+      </c>
+      <c r="H12">
+        <v>0.92400000000000004</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -731,8 +805,14 @@
       <c r="F13" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="G13">
+        <v>7074.09</v>
+      </c>
+      <c r="H13">
+        <v>0.70699999999999996</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -751,8 +831,14 @@
       <c r="F14" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="G14">
+        <v>10156.235000000001</v>
+      </c>
+      <c r="H14">
+        <v>1.016</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -771,8 +857,14 @@
       <c r="F15" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G15">
+        <v>14011.459000000001</v>
+      </c>
+      <c r="H15">
+        <v>1.401</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -791,8 +883,14 @@
       <c r="F16" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="G16">
+        <v>12328.22</v>
+      </c>
+      <c r="H16">
+        <v>1.2330000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -811,8 +909,14 @@
       <c r="F17" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G17">
+        <v>11575.291999999999</v>
+      </c>
+      <c r="H17">
+        <v>1.1579999999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
@@ -831,8 +935,14 @@
       <c r="F18" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G18">
+        <v>13557.700999999999</v>
+      </c>
+      <c r="H18">
+        <v>1.3560000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
@@ -851,8 +961,14 @@
       <c r="F19" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="G19">
+        <v>7339.2049999999999</v>
+      </c>
+      <c r="H19">
+        <v>0.73399999999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
@@ -871,8 +987,14 @@
       <c r="F20" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="G20">
+        <v>12526.308000000001</v>
+      </c>
+      <c r="H20">
+        <v>1.2529999999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
@@ -891,8 +1013,14 @@
       <c r="F21" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" ht="12.5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G21">
+        <v>15052.763000000001</v>
+      </c>
+      <c r="H21">
+        <v>1.5049999999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
@@ -911,8 +1039,14 @@
       <c r="F22" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="G22">
+        <v>11011.726000000001</v>
+      </c>
+      <c r="H22">
+        <v>1.101</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
@@ -930,6 +1064,12 @@
       </c>
       <c r="F23" t="s">
         <v>9</v>
+      </c>
+      <c r="G23">
+        <v>16063.66</v>
+      </c>
+      <c r="H23">
+        <v>1.6060000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>